<commit_message>
passive ability example [axe counter helix]
</commit_message>
<xml_diff>
--- a/excels/技能表.xlsx
+++ b/excels/技能表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\x-template\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60FC55D6-005A-4E42-A2B7-41A104837974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{517552AB-21D5-49BB-9AEE-913111016162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{12E03100-0083-4591-82B6-AE44D6148A4E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="84">
   <si>
     <t>DOTA_ABILITY_BEHAVIOR_POINT | DOTA_ABILITY_BEHAVIOR_AOE</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -296,15 +296,66 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>examples/abilities/crystal_nova_x.lua</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>技能键值</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>键值描述</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>counter_helix_x</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>反击螺旋</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>受到一定次数攻击后，斧王就会做出螺旋反击，对附近所有敌方单位造成纯粹伤害。</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>预载资源</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Precache</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage 75 110 145 180</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>伤害</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>radius 275</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>范围</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>hit_count 7 6 5 4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>所需攻击次数</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>axe_counter_helix</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+	"soundfile"	"soundevents/game_sounds_heroes/game_sounds_axe.vsndevts"
+	"particle"	"particles/units/heroes/hero_axe/axe_counterhelix_ad.vpcf"
+}</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -397,7 +448,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -408,6 +459,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -723,10 +777,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9E96040-265A-4A93-876C-FCCB37D3CA62}">
-  <dimension ref="A1:AI3"/>
+  <dimension ref="A1:AJ4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AA4" sqref="AA4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -754,7 +808,7 @@
     <col min="26" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>67</v>
       </c>
@@ -772,10 +826,10 @@
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>71</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>62</v>
@@ -813,8 +867,11 @@
       <c r="AI1" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="AJ1" s="5" t="s">
+        <v>74</v>
+      </c>
     </row>
-    <row r="2" spans="1:35" s="3" customFormat="1" ht="21.45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:36" s="3" customFormat="1" ht="21.45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>50</v>
       </c>
@@ -920,8 +977,11 @@
       <c r="AI2" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="AJ2" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
-    <row r="3" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>68</v>
       </c>
@@ -934,8 +994,9 @@
       <c r="D3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>69</v>
+      <c r="E3" s="5" t="str">
+        <f>"examples/abilities/"&amp;A3&amp;".lua"</f>
+        <v>examples/abilities/crystal_nova_x.lua</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>18</v>
@@ -1002,6 +1063,51 @@
       </c>
       <c r="AI3" s="1">
         <v>0.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="5" t="str">
+        <f>"examples/abilities/"&amp;A4&amp;".lua"</f>
+        <v>examples/abilities/counter_helix_x.lua</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="X4" s="1">
+        <v>4</v>
+      </c>
+      <c r="AA4" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AJ4" s="6" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
a complex ability example [tiny toss]
</commit_message>
<xml_diff>
--- a/excels/技能表.xlsx
+++ b/excels/技能表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\x-template\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{517552AB-21D5-49BB-9AEE-913111016162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E6BD51-3A27-4406-985B-9F329F4CCBF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{12E03100-0083-4591-82B6-AE44D6148A4E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="102">
   <si>
     <t>DOTA_ABILITY_BEHAVIOR_POINT | DOTA_ABILITY_BEHAVIOR_AOE</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -356,6 +356,79 @@
 	"soundfile"	"soundevents/game_sounds_heroes/game_sounds_axe.vsndevts"
 	"particle"	"particles/units/heroes/hero_axe/axe_counterhelix_ad.vpcf"
 }</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>tiny_toss_x</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>投掷</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ability_lua</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>duration 1.1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>持续事件</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>grab_radius 275</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>被投掷者额外伤害</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>toss_damage 200 250 300 350</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>投掷伤害</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>tiny_toss</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+            "particle"  "particles/units/heroes/hero_tiny/tiny_toss_blur.vpcf"
+		}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>技能伤害类型</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AbilityUnitDamageType</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>DAMAGE_TYPE_MAGICAL</t>
+  </si>
+  <si>
+    <t>DAMAGE_TYPE_MAGICAL</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>DAMAGE_TYPE_PURE</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>投掷的技能描述！（懒得去找了）</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>bonus_damage_pct 30 60 90</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -777,10 +850,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9E96040-265A-4A93-876C-FCCB37D3CA62}">
-  <dimension ref="A1:AJ4"/>
+  <dimension ref="A1:AK5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AA4" sqref="AA4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -805,10 +881,12 @@
     <col min="21" max="22" width="15.640625" style="1" customWidth="1"/>
     <col min="23" max="24" width="8.7109375" style="1"/>
     <col min="25" max="25" width="16.78515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="8.7109375" style="1"/>
+    <col min="26" max="36" width="8.7109375" style="1"/>
+    <col min="37" max="37" width="16.640625" style="1" customWidth="1"/>
+    <col min="38" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>67</v>
       </c>
@@ -846,32 +924,35 @@
       <c r="AB1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AJ1" s="5" t="s">
+      <c r="AK1" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:36" s="3" customFormat="1" ht="21.45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:37" s="3" customFormat="1" ht="21.45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>50</v>
       </c>
@@ -957,31 +1038,34 @@
         <v>29</v>
       </c>
       <c r="AC2" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="AD2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="AE2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AE2" s="3" t="s">
+      <c r="AF2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AF2" s="3" t="s">
+      <c r="AG2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AG2" s="3" t="s">
+      <c r="AH2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AH2" s="3" t="s">
+      <c r="AI2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="AI2" s="3" t="s">
+      <c r="AJ2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="AJ2" s="3" t="s">
+      <c r="AK2" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:37" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>68</v>
       </c>
@@ -1055,17 +1139,20 @@
       <c r="AB3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="AC3" s="1" t="s">
+      <c r="AC3" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AH3" s="1">
+      <c r="AI3" s="1">
         <v>700</v>
       </c>
-      <c r="AI3" s="1">
+      <c r="AJ3" s="1">
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:37" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>71</v>
       </c>
@@ -1106,8 +1193,80 @@
       <c r="AA4" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="AJ4" s="6" t="s">
+      <c r="AC4" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="AK4" s="6" t="s">
         <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" s="5" t="str">
+        <f>"examples/abilities/"&amp;A5&amp;".lua"</f>
+        <v>examples/abilities/tiny_toss_x.lua</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="X5" s="1">
+        <v>4</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>10</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>70</v>
+      </c>
+      <c r="AA5" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AI5" s="1">
+        <v>1200</v>
+      </c>
+      <c r="AJ5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK5" s="6" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>